<commit_message>
Added Procfile and added gunicorn to requirements.txt
</commit_message>
<xml_diff>
--- a/app/static/images/One Solution Per Day.xlsx
+++ b/app/static/images/One Solution Per Day.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgott\Desktop\Coding\Coding_Temple\capstone-flask\app\static\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C47BD1-76FC-4604-98AB-D6F7190DE8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41CFC6A-D0FD-4C9A-88A0-029ACF641BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="588" windowWidth="22488" windowHeight="11112" xr2:uid="{04D6D47B-2052-4252-9814-11BC6B9677A5}"/>
+    <workbookView xWindow="1260" yWindow="132" windowWidth="17280" windowHeight="8004" xr2:uid="{04D6D47B-2052-4252-9814-11BC6B9677A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDD53B7-8FEE-489E-880E-83AB7AFEDA8D}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
hardcoded project of the day and removed for loop through projects to match with today's date
</commit_message>
<xml_diff>
--- a/app/static/images/One Solution Per Day.xlsx
+++ b/app/static/images/One Solution Per Day.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgott\Desktop\Coding\Coding_Temple\capstone-flask\app\static\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41CFC6A-D0FD-4C9A-88A0-029ACF641BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41B6ED2-CCD7-4ABB-9522-7E13D0D50097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="132" windowWidth="17280" windowHeight="8004" xr2:uid="{04D6D47B-2052-4252-9814-11BC6B9677A5}"/>
+    <workbookView xWindow="72" yWindow="5256" windowWidth="22968" windowHeight="6660" xr2:uid="{04D6D47B-2052-4252-9814-11BC6B9677A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,9 +188,6 @@
     <t>http://www.bethematch.com</t>
   </si>
   <si>
-    <t>{{ url_for('static', filename='images/organ.png') }}</t>
-  </si>
-  <si>
     <t>{{ url_for('static', filename='images/child_hunger.avif') }}</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>'problem': 'According to Yelp data,  97,966 businesses closed during the pandemic.', 'action': 'Buy something locally that you would usually go online for.', 'goal': '3000 Local Purchases', 'resource': 'https://sustainableconnections.org/why-buy-local/', 'image_link': "{{ url_for('static', filename='images/buy_local.png') }}"}, {'target_date': '2022-08-01', 'problem': 'Common decency is in short supply.', 'action': 'Do something nice for a stranger. Let someone merge. Hold a door. Offer up a positive example.', 'goal': '5000 Kind Gestures', 'resource': 'https://evc.ucsd.edu/about/ARCC.html', 'image_link': "{{ url_for('static', filename='images/Civility.png') }}"}, {'target_date': '2022-07-31', 'problem': 'Democracy is the worst sytem out there, except for all the others.', 'action': 'Find someone in your sphere who is not currently registered to vote and help them get registered today.', 'goal': '5000 Voter Registrations', 'resource': 'https://www.usa.gov/voter-registration', 'image_link': "{{ url_for('static', filename='images/vote.webp') }}"}, {'target_date': '2022-07-30', 'problem': 'Many women with young children end up in shelters due to abuse, neglect, or other challenges.', 'action': "Donate to women's shelter. (clothes, baby supplies, diapers)", 'goal': '2500 Donations', 'resource': 'https://www.thehotline.org/', 'image_link': "{{ url_for('static', filename='images/shelter.jpg') }}"}, {'target_date': '2022-07-29', 'problem': 'Over 10% of Americans, including 12 million children, struggle with food insecurity.', 'action': 'Donate to a food pantry.', 'goal': '3000 Donations', 'resource': 'https://hungerandhealth.feedingamerica.org/understand-food-insecurity/', 'image_link': "{{ url_for('static', filename='images/child_hunger.avif') }}"}, {'target_date': '2022-07-28', 'problem': 'Many patients die while still waiting for needed donor organs due to lack of supply.', 'action': 'Sign up to be an organ donor.', 'goal': '2000 Organ Donation Registrations', 'resource': 'http://www.bethematch.com', 'image_link': "{{ url_for('static', filename='images/organ.png') }}"}, {'target_date': '2022-07-27', 'problem': 'Blood supplies are low in many parts of the country and world.', 'action': 'Make an appointment to donate blood.', 'goal': '1500 Donations', 'resource': 'https://www.redcross.org/?cid=generic&amp;med=cpc&amp;source=google&amp;scode=RSG00000E017&amp;gclid=Cj0KCQjw8uOWBhDXARIsAOxKJ2EniDYkGct5vQyk4ILNO4Ovi783nwYSh1AzzviqBO7GT1v0v48xN_saAjLVEALw_wcB&amp;gclsrc=aw.ds', 'image_link': "{{ url_for('static', filename='images/blood.jpg') }}"}  ... displaying 10 of 12 total bound parameter sets ...  {'target_date': '2022-07-24', 'problem': 'Many elderly are feeling isolated during the pandemic.', 'action': 'Call an elderly member of your family today.', 'goal': '3000 Phone Calls', 'resource': 'https://www.cdc.gov/aging/publications/features/lonely-older-adults.html#:~:text=Older%20adults%20are%20at%20increased,the%20amount%20of%20social%20contact.', 'image_link': "{{ url_for('static', filename='images/elderly.jfif') }}"}, {'target_date': '2022-07-20', 'problem': '', 'action': '', 'goal': '', 'resource': '', 'image_link': "{{ url_for('static', filename='images/') }}"})]</t>
+  </si>
+  <si>
+    <t>{{ url_for('static', filename='images/organ.jpg') }}</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDD53B7-8FEE-489E-880E-83AB7AFEDA8D}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>44</v>
@@ -812,7 +812,7 @@
         <v>50</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -828,10 +828,10 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -847,7 +847,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>43</v>
@@ -866,7 +866,7 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>42</v>
@@ -878,17 +878,17 @@
         <v>44723</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -904,10 +904,10 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -923,10 +923,10 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -935,14 +935,14 @@
         <v>44726</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>45</v>
@@ -959,10 +959,10 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -978,10 +978,10 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -990,13 +990,13 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>